<commit_message>
Tercer commit nuevos ajustes de variables y data
</commit_message>
<xml_diff>
--- a/Data/DataPrimerProcesamiento .xlsx
+++ b/Data/DataPrimerProcesamiento .xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83000ACE-B3A5-4890-BC47-F42B648C566E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A50291E-F4B2-48B4-AF5F-B33641A57C8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,6 +913,106 @@
         <v>40</v>
       </c>
     </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>